<commit_message>
sprint-9 tasks codereview changes
</commit_message>
<xml_diff>
--- a/Exc2/FURPS_table.xlsx
+++ b/Exc2/FURPS_table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A116215228\IdeaProjects\Yandex\YP-sprint-9\Exc2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{068318E0-66D3-4698-8558-FDE78917A515}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8EB209-8566-49AE-B4D9-AA71853AE6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-51705" yWindow="-5520" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25905" yWindow="-5520" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>Код</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Необходимо защищать данные передающиеся по сети с помощью механизмов шифрования трафика</t>
   </si>
   <si>
-    <t>Основная задача цифровизации</t>
-  </si>
-  <si>
     <t>Централизованный расчёт ставок</t>
   </si>
   <si>
@@ -142,20 +139,44 @@
     <t>Рефакторинг системы</t>
   </si>
   <si>
-    <t>Необходимо в дальнейшем перейти на микросервисную архитектуру для возможности эффективного масштабирования и геолоцирования</t>
-  </si>
-  <si>
     <t>Экспертиза персонала</t>
   </si>
   <si>
     <t>Нужно убедиться что персонал готов работать с поставленными задачами используя условные технологии</t>
+  </si>
+  <si>
+    <t>Клиент может открыть страницу веб-сайта и подать заявку на депозит онлайн. Менеджер по депозитным процессам обрабатывает заявки в бек-офисе, подтверждая условия депозита в АБС банка</t>
+  </si>
+  <si>
+    <t>Просмотр и подача заявки на кредит на сайте</t>
+  </si>
+  <si>
+    <t>Клиент может открыть страницу веб-сайта и подать заявку на кредит онлайн. Менеджер по кредитным процессам обрабатывает заявки в бек-офисе, подтверждая условия кредита в АБС банка</t>
+  </si>
+  <si>
+    <t>Документация</t>
+  </si>
+  <si>
+    <t>Необходимо разработать документацию для улучшения процессов компании и передачи знаний</t>
+  </si>
+  <si>
+    <t>Внедрение Kafka</t>
+  </si>
+  <si>
+    <t>Необходимо использовать kafka в качестве брокера сообщений для улучшения надежности, производительности и отзывчивости системы</t>
+  </si>
+  <si>
+    <t>Необходимо максимально переиспользовать технологии которые уже используются в банке (MS SQL, Oracle) а так же языки программирования (Java, .NET, Python)</t>
+  </si>
+  <si>
+    <t>Необходимо в дальнейшем перейти на микросервисную архитектуру для возможности эффективного масштабирования и геолоцирования. Так же необходимо внедрить брокер сообщений kafka. Текущая платформа интернет-банка не совместима с Kafka</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -176,8 +197,17 @@
       <color theme="0"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Liberation Sans"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +232,12 @@
         <bgColor theme="4" tint="-0.249977111117893"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -304,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -328,26 +364,47 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -576,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.44140625" defaultRowHeight="13.2"/>
@@ -606,104 +663,104 @@
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="10"/>
-    </row>
-    <row r="5" spans="2:4" ht="41.4" customHeight="1">
+      <c r="D4" s="14"/>
+    </row>
+    <row r="5" spans="2:4" ht="81.599999999999994" customHeight="1">
       <c r="B5" s="2"/>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="45.6" customHeight="1">
+      <c r="D5" s="16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="90" customHeight="1">
       <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>20</v>
+      <c r="C6" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="96.6" customHeight="1">
       <c r="B7" s="2"/>
       <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="30" customHeight="1">
       <c r="B8" s="5"/>
       <c r="C8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>27</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="30" customHeight="1">
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="14"/>
     </row>
     <row r="10" spans="2:4" ht="38.4" customHeight="1">
       <c r="B10" s="2"/>
       <c r="C10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="41.4" customHeight="1">
       <c r="B11" s="5"/>
       <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="30" customHeight="1">
       <c r="B12" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="14"/>
     </row>
     <row r="13" spans="2:4" ht="30" customHeight="1">
-      <c r="B13" s="11"/>
-      <c r="C13" s="15" t="s">
+      <c r="B13" s="9"/>
+      <c r="C13" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="30" customHeight="1">
-      <c r="B14" s="11"/>
-      <c r="C14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>32</v>
+      <c r="B14" s="9"/>
+      <c r="C14" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="30" customHeight="1">
       <c r="B15" s="5"/>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="11" t="s">
         <v>18</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -714,88 +771,117 @@
       <c r="B16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="10"/>
+      <c r="D16" s="14"/>
     </row>
     <row r="17" spans="1:4" ht="36.6" customHeight="1">
       <c r="B17" s="2"/>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>30</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39" customHeight="1">
       <c r="B18" s="5"/>
       <c r="C18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1">
       <c r="B19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="C19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4" ht="47.4" customHeight="1">
       <c r="B20" s="2"/>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="4" t="s">
+    </row>
+    <row r="21" spans="1:4" ht="47.4" customHeight="1">
+      <c r="B21" s="9"/>
+      <c r="C21" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="22" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="42.6" customHeight="1">
+      <c r="B22" s="5"/>
+      <c r="C22" s="11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="42.6" customHeight="1">
-      <c r="B21" s="5"/>
-      <c r="C21" s="3" t="s">
+      <c r="D22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" customHeight="1">
-      <c r="B22" s="2" t="s">
+    </row>
+    <row r="23" spans="1:4" ht="30" customHeight="1">
+      <c r="B23" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C23" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="1:4" ht="55.2" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="47.4" customHeight="1">
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:4" ht="99.6" customHeight="1">
       <c r="A24" s="8"/>
       <c r="B24" s="5"/>
       <c r="C24" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="55.2" customHeight="1">
+      <c r="A25" s="8"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="55.2" customHeight="1">
+      <c r="A26" s="8"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="47.4" customHeight="1">
+      <c r="A27" s="8"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C12:D12"/>
@@ -803,6 +889,6 @@
     <mergeCell ref="C19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51181102362204689" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>